<commit_message>
documentation and update of filesystem.xls
</commit_message>
<xml_diff>
--- a/filesystem.xlsx
+++ b/filesystem.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\rust\didentity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\rust\fstore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935DD655-2A81-469D-9A7A-C1A31F4D0EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5FCC58-C8A3-49DB-8CC9-F340BC3C3012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="750" windowWidth="19440" windowHeight="15600" xr2:uid="{D8B445F8-E14E-46C9-ABB7-1D49E1DA020C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D8B445F8-E14E-46C9-ABB7-1D49E1DA020C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Size</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Data Block</t>
   </si>
   <si>
-    <t>size of chunk</t>
-  </si>
-  <si>
     <t>address of next chunk</t>
   </si>
   <si>
@@ -96,15 +93,9 @@
     <t>total size of data</t>
   </si>
   <si>
-    <t>sizeof data chunk</t>
-  </si>
-  <si>
     <t>checksum</t>
   </si>
   <si>
-    <t>1byte</t>
-  </si>
-  <si>
     <t>64b</t>
   </si>
   <si>
@@ -114,27 +105,6 @@
     <t>Sequential Binary File Format</t>
   </si>
   <si>
-    <t>Address Block</t>
-  </si>
-  <si>
-    <t>can hold 1023 block addresses, plus the position to next address</t>
-  </si>
-  <si>
-    <t>previous address block</t>
-  </si>
-  <si>
-    <t>64bx1022</t>
-  </si>
-  <si>
-    <t>1022 addresses</t>
-  </si>
-  <si>
-    <t>next address block</t>
-  </si>
-  <si>
-    <t>65536b[]</t>
-  </si>
-  <si>
     <t>deletes can nullify this data</t>
   </si>
   <si>
@@ -147,13 +117,22 @@
     <t>deleted</t>
   </si>
   <si>
-    <t>allocated</t>
-  </si>
-  <si>
-    <t>has previous chunk</t>
-  </si>
-  <si>
     <t>size of string</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>the data</t>
+  </si>
+  <si>
+    <t>Allocated</t>
+  </si>
+  <si>
+    <t>size of data</t>
+  </si>
+  <si>
+    <t>checksum, 32b probably sufficient 0 if not used</t>
   </si>
 </sst>
 </file>
@@ -505,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5FA646-0B59-4576-B82F-11280CEFE4EA}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C19:C20"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +499,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -551,7 +530,7 @@
         <v>5</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -559,12 +538,12 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -579,144 +558,93 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="J8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9">
-        <v>4</v>
-      </c>
-      <c r="K9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J10">
-        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
         <v>29</v>
-      </c>
-      <c r="B23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>